<commit_message>
HW1 Weapon Review and Updates
Pretty solid. Ints vs hw1 corvs still need work though.

Spent most of this week doing tones of tests.
</commit_message>
<xml_diff>
--- a/Balance Info/2.3 Players Patch - Swarm Balancing 120217.xlsx
+++ b/Balance Info/2.3 Players Patch - Swarm Balancing 120217.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Offline Files\GameStuff\HomeworldRemastered\Information\Balance\Old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Homeworld Remastered Patch Beta\HomeworldRM\Git\2.3\Balance Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="2.3 Patch Balancing" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="79">
   <si>
     <t>total</t>
   </si>
@@ -223,15 +224,61 @@
   <si>
     <t>Heavy Corvs .58</t>
   </si>
+  <si>
+    <t>Laser vs</t>
+  </si>
+  <si>
+    <t>laser win</t>
+  </si>
+  <si>
+    <t>ass win</t>
+  </si>
+  <si>
+    <t>avg:</t>
+  </si>
+  <si>
+    <t>Pulsar vs kus ass</t>
+  </si>
+  <si>
+    <t>pulsar vs tai ass</t>
+  </si>
+  <si>
+    <t>Kus Heavy vs Assault Frigs</t>
+  </si>
+  <si>
+    <t>Kus Heavy vs Torps</t>
+  </si>
+  <si>
+    <t>torp win</t>
+  </si>
+  <si>
+    <t>b8 wip 7/26</t>
+  </si>
+  <si>
+    <t>K HC 45</t>
+  </si>
+  <si>
+    <t>H Puls 45</t>
+  </si>
+  <si>
+    <t>V Miss 60</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -293,16 +340,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HH36"/>
+  <dimension ref="A1:JH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="HY1" workbookViewId="0">
+      <selection activeCell="IR5" sqref="IR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,20 +694,32 @@
     <col min="203" max="206" width="5.7109375" style="2" customWidth="1"/>
     <col min="208" max="211" width="5.7109375" style="1" customWidth="1"/>
     <col min="213" max="216" width="5.7109375" style="1" customWidth="1"/>
+    <col min="220" max="223" width="5.7109375" style="1" customWidth="1"/>
+    <col min="225" max="228" width="5.7109375" style="1" customWidth="1"/>
+    <col min="230" max="233" width="5.7109375" style="7" customWidth="1"/>
+    <col min="234" max="234" width="9.140625" style="7"/>
+    <col min="235" max="243" width="5.7109375" style="7" customWidth="1"/>
+    <col min="244" max="244" width="9.140625" style="7"/>
+    <col min="245" max="248" width="5.7109375" style="7" customWidth="1"/>
+    <col min="250" max="253" width="5.7109375" style="1" customWidth="1"/>
+    <col min="255" max="258" width="5.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="5.7109375" style="4" customWidth="1"/>
+    <col min="260" max="263" width="5.7109375" style="1" customWidth="1"/>
+    <col min="265" max="268" width="5.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:268" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
@@ -663,196 +729,241 @@
       <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
       <c r="S1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
       <c r="AC1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="AD1" s="8"/>
       <c r="AE1" s="8"/>
       <c r="AF1" s="8"/>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
       <c r="AM1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AN1" s="8"/>
       <c r="AO1" s="8"/>
       <c r="AP1" s="8"/>
-      <c r="AR1" s="7" t="s">
+      <c r="AR1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="BI1" s="7">
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="BI1" s="9">
         <v>0.5</v>
       </c>
-      <c r="BJ1" s="7"/>
-      <c r="BK1" s="7"/>
-      <c r="BL1" s="7"/>
-      <c r="BN1" s="7">
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BN1" s="9">
         <v>0.5</v>
       </c>
-      <c r="BO1" s="7"/>
-      <c r="BP1" s="7"/>
-      <c r="BQ1" s="7"/>
-      <c r="BS1" s="7"/>
-      <c r="BT1" s="7"/>
-      <c r="BU1" s="7"/>
-      <c r="BV1" s="7"/>
-      <c r="BX1" s="7"/>
-      <c r="BY1" s="7"/>
-      <c r="BZ1" s="7"/>
-      <c r="CA1" s="7"/>
-      <c r="CC1" s="9" t="s">
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9"/>
+      <c r="BV1" s="9"/>
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CC1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="CD1" s="9"/>
-      <c r="CF1" s="7"/>
-      <c r="CG1" s="7"/>
-      <c r="CH1" s="7"/>
-      <c r="CI1" s="7"/>
-      <c r="CK1" s="7"/>
-      <c r="CL1" s="7"/>
-      <c r="CM1" s="7"/>
-      <c r="CN1" s="7"/>
+      <c r="CD1" s="10"/>
+      <c r="CF1" s="9"/>
+      <c r="CG1" s="9"/>
+      <c r="CH1" s="9"/>
+      <c r="CI1" s="9"/>
+      <c r="CK1" s="9"/>
+      <c r="CL1" s="9"/>
+      <c r="CM1" s="9"/>
+      <c r="CN1" s="9"/>
       <c r="CO1" s="3"/>
-      <c r="CP1" s="7"/>
-      <c r="CQ1" s="7"/>
-      <c r="CR1" s="7"/>
-      <c r="CS1" s="7"/>
-      <c r="CU1" s="7"/>
-      <c r="CV1" s="7"/>
-      <c r="CW1" s="7"/>
-      <c r="CX1" s="7"/>
+      <c r="CP1" s="9"/>
+      <c r="CQ1" s="9"/>
+      <c r="CR1" s="9"/>
+      <c r="CS1" s="9"/>
+      <c r="CU1" s="9"/>
+      <c r="CV1" s="9"/>
+      <c r="CW1" s="9"/>
+      <c r="CX1" s="9"/>
       <c r="CY1" s="3"/>
-      <c r="CZ1" s="7"/>
-      <c r="DA1" s="7"/>
-      <c r="DB1" s="7"/>
-      <c r="DC1" s="7"/>
-      <c r="DE1" s="7"/>
-      <c r="DF1" s="7"/>
-      <c r="DG1" s="7"/>
-      <c r="DH1" s="7"/>
+      <c r="CZ1" s="9"/>
+      <c r="DA1" s="9"/>
+      <c r="DB1" s="9"/>
+      <c r="DC1" s="9"/>
+      <c r="DE1" s="9"/>
+      <c r="DF1" s="9"/>
+      <c r="DG1" s="9"/>
+      <c r="DH1" s="9"/>
       <c r="DI1" s="6"/>
-      <c r="DK1" s="7"/>
-      <c r="DL1" s="7"/>
-      <c r="DM1" s="7"/>
-      <c r="DN1" s="7"/>
-      <c r="DP1" s="7"/>
-      <c r="DQ1" s="7"/>
-      <c r="DR1" s="7"/>
-      <c r="DS1" s="7"/>
-      <c r="DU1" s="7"/>
-      <c r="DV1" s="7"/>
-      <c r="DW1" s="7"/>
-      <c r="DX1" s="7"/>
-      <c r="DZ1" s="7"/>
-      <c r="EA1" s="7"/>
-      <c r="EB1" s="7"/>
-      <c r="EC1" s="7"/>
-      <c r="EE1" s="7"/>
-      <c r="EF1" s="7"/>
-      <c r="EG1" s="7"/>
-      <c r="EH1" s="7"/>
-      <c r="EJ1" s="7"/>
-      <c r="EK1" s="7"/>
-      <c r="EL1" s="7"/>
-      <c r="EM1" s="7"/>
+      <c r="DK1" s="9"/>
+      <c r="DL1" s="9"/>
+      <c r="DM1" s="9"/>
+      <c r="DN1" s="9"/>
+      <c r="DP1" s="9"/>
+      <c r="DQ1" s="9"/>
+      <c r="DR1" s="9"/>
+      <c r="DS1" s="9"/>
+      <c r="DU1" s="9"/>
+      <c r="DV1" s="9"/>
+      <c r="DW1" s="9"/>
+      <c r="DX1" s="9"/>
+      <c r="DZ1" s="9"/>
+      <c r="EA1" s="9"/>
+      <c r="EB1" s="9"/>
+      <c r="EC1" s="9"/>
+      <c r="EE1" s="9"/>
+      <c r="EF1" s="9"/>
+      <c r="EG1" s="9"/>
+      <c r="EH1" s="9"/>
+      <c r="EJ1" s="9"/>
+      <c r="EK1" s="9"/>
+      <c r="EL1" s="9"/>
+      <c r="EM1" s="9"/>
       <c r="EP1" t="s">
         <v>45</v>
       </c>
-      <c r="ES1" s="7">
+      <c r="ES1" s="9">
         <v>0.6</v>
       </c>
-      <c r="ET1" s="7"/>
-      <c r="EU1" s="7"/>
-      <c r="EV1" s="7"/>
-      <c r="EX1" s="7"/>
-      <c r="EY1" s="7"/>
-      <c r="EZ1" s="7"/>
-      <c r="FA1" s="7"/>
-      <c r="FC1" s="7"/>
-      <c r="FD1" s="7"/>
-      <c r="FE1" s="7"/>
-      <c r="FF1" s="7"/>
-      <c r="FH1" s="7"/>
-      <c r="FI1" s="7"/>
-      <c r="FJ1" s="7"/>
-      <c r="FK1" s="7"/>
-      <c r="FM1" s="7"/>
-      <c r="FN1" s="7"/>
-      <c r="FO1" s="7"/>
-      <c r="FP1" s="7"/>
-      <c r="FR1" s="7"/>
-      <c r="FS1" s="7"/>
-      <c r="FT1" s="7"/>
-      <c r="FU1" s="7"/>
+      <c r="ET1" s="9"/>
+      <c r="EU1" s="9"/>
+      <c r="EV1" s="9"/>
+      <c r="EX1" s="9"/>
+      <c r="EY1" s="9"/>
+      <c r="EZ1" s="9"/>
+      <c r="FA1" s="9"/>
+      <c r="FC1" s="9"/>
+      <c r="FD1" s="9"/>
+      <c r="FE1" s="9"/>
+      <c r="FF1" s="9"/>
+      <c r="FH1" s="9"/>
+      <c r="FI1" s="9"/>
+      <c r="FJ1" s="9"/>
+      <c r="FK1" s="9"/>
+      <c r="FM1" s="9"/>
+      <c r="FN1" s="9"/>
+      <c r="FO1" s="9"/>
+      <c r="FP1" s="9"/>
+      <c r="FR1" s="9"/>
+      <c r="FS1" s="9"/>
+      <c r="FT1" s="9"/>
+      <c r="FU1" s="9"/>
       <c r="GA1" s="8" t="s">
         <v>54</v>
       </c>
       <c r="GB1" s="8"/>
       <c r="GC1" s="8"/>
       <c r="GD1" s="8"/>
-      <c r="GF1" s="7" t="s">
+      <c r="GF1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="GG1" s="7"/>
-      <c r="GH1" s="7"/>
-      <c r="GI1" s="7"/>
-      <c r="GK1" s="7" t="s">
+      <c r="GG1" s="9"/>
+      <c r="GH1" s="9"/>
+      <c r="GI1" s="9"/>
+      <c r="GK1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="GL1" s="7"/>
-      <c r="GM1" s="7"/>
-      <c r="GN1" s="7"/>
-      <c r="GP1" s="7" t="s">
+      <c r="GL1" s="9"/>
+      <c r="GM1" s="9"/>
+      <c r="GN1" s="9"/>
+      <c r="GP1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="GQ1" s="7"/>
-      <c r="GR1" s="7"/>
-      <c r="GS1" s="7"/>
+      <c r="GQ1" s="9"/>
+      <c r="GR1" s="9"/>
+      <c r="GS1" s="9"/>
       <c r="GU1" s="8" t="s">
         <v>58</v>
       </c>
       <c r="GV1" s="8"/>
       <c r="GW1" s="8"/>
       <c r="GX1" s="8"/>
-      <c r="GZ1" s="7" t="s">
+      <c r="GZ1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="HA1" s="7"/>
-      <c r="HB1" s="7"/>
-      <c r="HC1" s="7"/>
-      <c r="HE1" s="7" t="s">
+      <c r="HA1" s="9"/>
+      <c r="HB1" s="9"/>
+      <c r="HC1" s="9"/>
+      <c r="HE1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="HF1" s="7"/>
-      <c r="HG1" s="7"/>
-      <c r="HH1" s="7"/>
+      <c r="HF1" s="9"/>
+      <c r="HG1" s="9"/>
+      <c r="HH1" s="9"/>
+      <c r="HJ1" t="s">
+        <v>75</v>
+      </c>
+      <c r="HL1" s="9"/>
+      <c r="HM1" s="9"/>
+      <c r="HN1" s="9"/>
+      <c r="HO1" s="9"/>
+      <c r="HQ1" s="9"/>
+      <c r="HR1" s="9"/>
+      <c r="HS1" s="9"/>
+      <c r="HT1" s="9"/>
+      <c r="HV1" s="12"/>
+      <c r="HW1" s="12"/>
+      <c r="HX1" s="12"/>
+      <c r="HY1" s="12"/>
+      <c r="IA1" s="12"/>
+      <c r="IB1" s="12"/>
+      <c r="IC1" s="12"/>
+      <c r="ID1" s="12"/>
+      <c r="IE1" s="13"/>
+      <c r="IF1" s="12"/>
+      <c r="IG1" s="12"/>
+      <c r="IH1" s="12"/>
+      <c r="II1" s="12"/>
+      <c r="IK1" s="12"/>
+      <c r="IL1" s="12"/>
+      <c r="IM1" s="12"/>
+      <c r="IN1" s="12"/>
+      <c r="IP1" s="9"/>
+      <c r="IQ1" s="9"/>
+      <c r="IR1" s="9"/>
+      <c r="IS1" s="9"/>
+      <c r="IU1" s="9"/>
+      <c r="IV1" s="9"/>
+      <c r="IW1" s="9"/>
+      <c r="IX1" s="9"/>
+      <c r="IY1" s="3"/>
+      <c r="IZ1" s="9"/>
+      <c r="JA1" s="9"/>
+      <c r="JB1" s="9"/>
+      <c r="JC1" s="9"/>
+      <c r="JE1" s="9"/>
+      <c r="JF1" s="9"/>
+      <c r="JG1" s="9"/>
+      <c r="JH1" s="9"/>
     </row>
-    <row r="2" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:268" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
@@ -1213,8 +1324,98 @@
       <c r="HH2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="HM2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="HN2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="HO2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="HR2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="HS2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="HT2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="HW2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="HX2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="HY2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="IB2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="IC2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="ID2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="IG2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="IH2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="II2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="IL2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="IM2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="IN2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="IQ2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="IR2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="IS2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="IV2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="IW2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="IX2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="JA2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="JB2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="JC2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="JF2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="JG2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="JH2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <v>37</v>
       </c>
@@ -1488,8 +1689,62 @@
       <c r="HF3" s="1">
         <v>19</v>
       </c>
+      <c r="HL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="HM3" s="1">
+        <v>15</v>
+      </c>
+      <c r="HO3" s="1">
+        <v>130</v>
+      </c>
+      <c r="HQ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="HR3" s="1">
+        <v>21</v>
+      </c>
+      <c r="HT3" s="1">
+        <v>175</v>
+      </c>
+      <c r="HV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="HW3" s="7">
+        <v>46</v>
+      </c>
+      <c r="IA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="IC3" s="7">
+        <v>19</v>
+      </c>
+      <c r="IF3" s="7">
+        <v>1</v>
+      </c>
+      <c r="IG3" s="7">
+        <v>25</v>
+      </c>
+      <c r="IK3" s="7">
+        <v>1</v>
+      </c>
+      <c r="IM3" s="7">
+        <v>16</v>
+      </c>
+      <c r="IP3" s="1">
+        <v>1</v>
+      </c>
+      <c r="IU3" s="1">
+        <v>1</v>
+      </c>
+      <c r="IZ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="JE3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
         <v>30</v>
       </c>
@@ -1763,8 +2018,62 @@
       <c r="HF4" s="1">
         <v>17</v>
       </c>
+      <c r="HL4" s="1">
+        <v>2</v>
+      </c>
+      <c r="HN4" s="1">
+        <v>19</v>
+      </c>
+      <c r="HO4" s="1">
+        <v>117</v>
+      </c>
+      <c r="HQ4" s="1">
+        <v>2</v>
+      </c>
+      <c r="HR4" s="1">
+        <v>11</v>
+      </c>
+      <c r="HT4" s="1">
+        <v>210</v>
+      </c>
+      <c r="HV4" s="7">
+        <v>2</v>
+      </c>
+      <c r="HW4" s="7">
+        <v>52</v>
+      </c>
+      <c r="IA4" s="7">
+        <v>2</v>
+      </c>
+      <c r="IB4" s="7">
+        <v>24</v>
+      </c>
+      <c r="IF4" s="7">
+        <v>2</v>
+      </c>
+      <c r="IG4" s="7">
+        <v>7</v>
+      </c>
+      <c r="IK4" s="7">
+        <v>2</v>
+      </c>
+      <c r="IM4" s="7">
+        <v>17</v>
+      </c>
+      <c r="IP4" s="1">
+        <v>2</v>
+      </c>
+      <c r="IU4" s="1">
+        <v>2</v>
+      </c>
+      <c r="IZ4" s="1">
+        <v>2</v>
+      </c>
+      <c r="JE4" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>31</v>
       </c>
@@ -2035,8 +2344,62 @@
       <c r="HF5" s="1">
         <v>1</v>
       </c>
+      <c r="HL5" s="1">
+        <v>3</v>
+      </c>
+      <c r="HN5" s="1">
+        <v>13</v>
+      </c>
+      <c r="HO5" s="1">
+        <v>131</v>
+      </c>
+      <c r="HQ5" s="1">
+        <v>3</v>
+      </c>
+      <c r="HS5" s="1">
+        <v>13</v>
+      </c>
+      <c r="HT5" s="1">
+        <v>203</v>
+      </c>
+      <c r="HV5" s="7">
+        <v>3</v>
+      </c>
+      <c r="HW5" s="7">
+        <v>33</v>
+      </c>
+      <c r="IA5" s="7">
+        <v>3</v>
+      </c>
+      <c r="IB5" s="7">
+        <v>13</v>
+      </c>
+      <c r="IF5" s="7">
+        <v>3</v>
+      </c>
+      <c r="IG5" s="7">
+        <v>25</v>
+      </c>
+      <c r="IK5" s="7">
+        <v>3</v>
+      </c>
+      <c r="IM5" s="7">
+        <v>16</v>
+      </c>
+      <c r="IP5" s="1">
+        <v>3</v>
+      </c>
+      <c r="IU5" s="1">
+        <v>3</v>
+      </c>
+      <c r="IZ5" s="1">
+        <v>3</v>
+      </c>
+      <c r="JE5" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>5</v>
       </c>
@@ -2292,8 +2655,56 @@
       <c r="HG6" s="1">
         <v>10</v>
       </c>
+      <c r="HL6" s="1">
+        <v>4</v>
+      </c>
+      <c r="HM6" s="1">
+        <v>10</v>
+      </c>
+      <c r="HO6" s="1">
+        <v>136</v>
+      </c>
+      <c r="HQ6" s="1">
+        <v>4</v>
+      </c>
+      <c r="HR6" s="1">
+        <v>11</v>
+      </c>
+      <c r="HT6" s="1">
+        <v>199</v>
+      </c>
+      <c r="HV6" s="7">
+        <v>4</v>
+      </c>
+      <c r="IA6" s="7">
+        <v>4</v>
+      </c>
+      <c r="IC6" s="7">
+        <v>14</v>
+      </c>
+      <c r="IF6" s="7">
+        <v>4</v>
+      </c>
+      <c r="IG6" s="7">
+        <v>38</v>
+      </c>
+      <c r="IK6" s="7">
+        <v>4</v>
+      </c>
+      <c r="IP6" s="1">
+        <v>4</v>
+      </c>
+      <c r="IU6" s="1">
+        <v>4</v>
+      </c>
+      <c r="IZ6" s="1">
+        <v>4</v>
+      </c>
+      <c r="JE6" s="1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>45</v>
       </c>
@@ -2543,8 +2954,50 @@
       <c r="HF7" s="1">
         <v>15</v>
       </c>
+      <c r="HL7" s="1">
+        <v>5</v>
+      </c>
+      <c r="HM7" s="1">
+        <v>10</v>
+      </c>
+      <c r="HO7" s="1">
+        <v>141</v>
+      </c>
+      <c r="HQ7" s="1">
+        <v>5</v>
+      </c>
+      <c r="HV7" s="7">
+        <v>5</v>
+      </c>
+      <c r="IA7" s="7">
+        <v>5</v>
+      </c>
+      <c r="IC7" s="7">
+        <v>18</v>
+      </c>
+      <c r="IF7" s="7">
+        <v>5</v>
+      </c>
+      <c r="IG7" s="7">
+        <v>41</v>
+      </c>
+      <c r="IK7" s="7">
+        <v>5</v>
+      </c>
+      <c r="IP7" s="1">
+        <v>5</v>
+      </c>
+      <c r="IU7" s="1">
+        <v>5</v>
+      </c>
+      <c r="IZ7" s="1">
+        <v>5</v>
+      </c>
+      <c r="JE7" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:268" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>8</v>
       </c>
@@ -2749,8 +3202,41 @@
       <c r="HE8" s="1">
         <v>6</v>
       </c>
+      <c r="HL8" s="1">
+        <v>6</v>
+      </c>
+      <c r="HQ8" s="1">
+        <v>6</v>
+      </c>
+      <c r="HV8" s="7">
+        <v>6</v>
+      </c>
+      <c r="IA8" s="7">
+        <v>6</v>
+      </c>
+      <c r="IC8" s="7">
+        <v>4</v>
+      </c>
+      <c r="IF8" s="7">
+        <v>6</v>
+      </c>
+      <c r="IK8" s="7">
+        <v>6</v>
+      </c>
+      <c r="IP8" s="1">
+        <v>6</v>
+      </c>
+      <c r="IU8" s="1">
+        <v>6</v>
+      </c>
+      <c r="IZ8" s="1">
+        <v>6</v>
+      </c>
+      <c r="JE8" s="1">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>6</v>
       </c>
@@ -2946,8 +3432,41 @@
       <c r="HE9" s="1">
         <v>7</v>
       </c>
+      <c r="HL9" s="1">
+        <v>7</v>
+      </c>
+      <c r="HQ9" s="1">
+        <v>7</v>
+      </c>
+      <c r="HV9" s="7">
+        <v>7</v>
+      </c>
+      <c r="IA9" s="7">
+        <v>7</v>
+      </c>
+      <c r="IC9" s="7">
+        <v>12</v>
+      </c>
+      <c r="IF9" s="7">
+        <v>7</v>
+      </c>
+      <c r="IK9" s="7">
+        <v>7</v>
+      </c>
+      <c r="IP9" s="1">
+        <v>7</v>
+      </c>
+      <c r="IU9" s="1">
+        <v>7</v>
+      </c>
+      <c r="IZ9" s="1">
+        <v>7</v>
+      </c>
+      <c r="JE9" s="1">
+        <v>7</v>
+      </c>
     </row>
-    <row r="10" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <v>39</v>
       </c>
@@ -3122,8 +3641,41 @@
       <c r="HE10" s="1">
         <v>8</v>
       </c>
+      <c r="HL10" s="1">
+        <v>8</v>
+      </c>
+      <c r="HQ10" s="1">
+        <v>8</v>
+      </c>
+      <c r="HV10" s="7">
+        <v>8</v>
+      </c>
+      <c r="IA10" s="7">
+        <v>8</v>
+      </c>
+      <c r="IC10" s="7">
+        <v>17</v>
+      </c>
+      <c r="IF10" s="7">
+        <v>8</v>
+      </c>
+      <c r="IK10" s="7">
+        <v>8</v>
+      </c>
+      <c r="IP10" s="1">
+        <v>8</v>
+      </c>
+      <c r="IU10" s="1">
+        <v>8</v>
+      </c>
+      <c r="IZ10" s="1">
+        <v>8</v>
+      </c>
+      <c r="JE10" s="1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <v>4</v>
       </c>
@@ -3292,8 +3844,41 @@
       <c r="HE11" s="1">
         <v>9</v>
       </c>
+      <c r="HL11" s="1">
+        <v>9</v>
+      </c>
+      <c r="HQ11" s="1">
+        <v>9</v>
+      </c>
+      <c r="HV11" s="7">
+        <v>9</v>
+      </c>
+      <c r="IA11" s="7">
+        <v>9</v>
+      </c>
+      <c r="IC11" s="7">
+        <v>18</v>
+      </c>
+      <c r="IF11" s="7">
+        <v>9</v>
+      </c>
+      <c r="IK11" s="7">
+        <v>9</v>
+      </c>
+      <c r="IP11" s="1">
+        <v>9</v>
+      </c>
+      <c r="IU11" s="1">
+        <v>9</v>
+      </c>
+      <c r="IZ11" s="1">
+        <v>9</v>
+      </c>
+      <c r="JE11" s="1">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <v>36</v>
       </c>
@@ -3484,8 +4069,41 @@
       <c r="HE12" s="1">
         <v>10</v>
       </c>
+      <c r="HL12" s="1">
+        <v>10</v>
+      </c>
+      <c r="HQ12" s="1">
+        <v>10</v>
+      </c>
+      <c r="HV12" s="7">
+        <v>10</v>
+      </c>
+      <c r="IA12" s="7">
+        <v>10</v>
+      </c>
+      <c r="IC12" s="7">
+        <v>2</v>
+      </c>
+      <c r="IF12" s="7">
+        <v>10</v>
+      </c>
+      <c r="IK12" s="7">
+        <v>10</v>
+      </c>
+      <c r="IP12" s="1">
+        <v>10</v>
+      </c>
+      <c r="IU12" s="1">
+        <v>10</v>
+      </c>
+      <c r="IZ12" s="1">
+        <v>10</v>
+      </c>
+      <c r="JE12" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="13" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <v>35</v>
       </c>
@@ -3627,8 +4245,41 @@
       <c r="HE13" s="1">
         <v>11</v>
       </c>
+      <c r="HL13" s="1">
+        <v>11</v>
+      </c>
+      <c r="HQ13" s="1">
+        <v>11</v>
+      </c>
+      <c r="HV13" s="7">
+        <v>11</v>
+      </c>
+      <c r="IA13" s="7">
+        <v>11</v>
+      </c>
+      <c r="IC13" s="7">
+        <v>14</v>
+      </c>
+      <c r="IF13" s="7">
+        <v>11</v>
+      </c>
+      <c r="IK13" s="7">
+        <v>11</v>
+      </c>
+      <c r="IP13" s="1">
+        <v>11</v>
+      </c>
+      <c r="IU13" s="1">
+        <v>11</v>
+      </c>
+      <c r="IZ13" s="1">
+        <v>11</v>
+      </c>
+      <c r="JE13" s="1">
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <v>38</v>
       </c>
@@ -3770,8 +4421,41 @@
       <c r="HE14" s="1">
         <v>12</v>
       </c>
+      <c r="HL14" s="1">
+        <v>12</v>
+      </c>
+      <c r="HQ14" s="1">
+        <v>12</v>
+      </c>
+      <c r="HV14" s="7">
+        <v>12</v>
+      </c>
+      <c r="IA14" s="7">
+        <v>12</v>
+      </c>
+      <c r="IC14" s="7">
+        <v>6</v>
+      </c>
+      <c r="IF14" s="7">
+        <v>12</v>
+      </c>
+      <c r="IK14" s="7">
+        <v>12</v>
+      </c>
+      <c r="IP14" s="1">
+        <v>12</v>
+      </c>
+      <c r="IU14" s="1">
+        <v>12</v>
+      </c>
+      <c r="IZ14" s="1">
+        <v>12</v>
+      </c>
+      <c r="JE14" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="15" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <v>41</v>
       </c>
@@ -3910,8 +4594,41 @@
       <c r="HE15" s="1">
         <v>13</v>
       </c>
+      <c r="HL15" s="1">
+        <v>13</v>
+      </c>
+      <c r="HQ15" s="1">
+        <v>13</v>
+      </c>
+      <c r="HV15" s="7">
+        <v>13</v>
+      </c>
+      <c r="IA15" s="7">
+        <v>13</v>
+      </c>
+      <c r="IC15" s="7">
+        <v>12</v>
+      </c>
+      <c r="IF15" s="7">
+        <v>13</v>
+      </c>
+      <c r="IK15" s="7">
+        <v>13</v>
+      </c>
+      <c r="IP15" s="1">
+        <v>13</v>
+      </c>
+      <c r="IU15" s="1">
+        <v>13</v>
+      </c>
+      <c r="IZ15" s="1">
+        <v>13</v>
+      </c>
+      <c r="JE15" s="1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="16" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:268" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <v>35</v>
       </c>
@@ -4050,8 +4767,41 @@
       <c r="HE16" s="1">
         <v>14</v>
       </c>
+      <c r="HL16" s="1">
+        <v>14</v>
+      </c>
+      <c r="HQ16" s="1">
+        <v>14</v>
+      </c>
+      <c r="HV16" s="7">
+        <v>14</v>
+      </c>
+      <c r="IA16" s="7">
+        <v>14</v>
+      </c>
+      <c r="IC16" s="7">
+        <v>14</v>
+      </c>
+      <c r="IF16" s="7">
+        <v>14</v>
+      </c>
+      <c r="IK16" s="7">
+        <v>14</v>
+      </c>
+      <c r="IP16" s="1">
+        <v>14</v>
+      </c>
+      <c r="IU16" s="1">
+        <v>14</v>
+      </c>
+      <c r="IZ16" s="1">
+        <v>14</v>
+      </c>
+      <c r="JE16" s="1">
+        <v>14</v>
+      </c>
     </row>
-    <row r="17" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:265" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>17</v>
       </c>
@@ -4190,8 +4940,41 @@
       <c r="HE17" s="1">
         <v>15</v>
       </c>
+      <c r="HL17" s="1">
+        <v>15</v>
+      </c>
+      <c r="HQ17" s="1">
+        <v>15</v>
+      </c>
+      <c r="HV17" s="7">
+        <v>15</v>
+      </c>
+      <c r="IA17" s="7">
+        <v>15</v>
+      </c>
+      <c r="IC17" s="7">
+        <v>15</v>
+      </c>
+      <c r="IF17" s="7">
+        <v>15</v>
+      </c>
+      <c r="IK17" s="7">
+        <v>15</v>
+      </c>
+      <c r="IP17" s="1">
+        <v>15</v>
+      </c>
+      <c r="IU17" s="1">
+        <v>15</v>
+      </c>
+      <c r="IZ17" s="1">
+        <v>15</v>
+      </c>
+      <c r="JE17" s="1">
+        <v>15</v>
+      </c>
     </row>
-    <row r="18" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:265" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>26</v>
       </c>
@@ -4336,8 +5119,50 @@
       <c r="HH18" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="HL18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="HN18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="HO18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="HQ18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="HS18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="HT18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="HV18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="IA18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="IF18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="IK18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="IP18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="IU18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="IZ18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="JE18" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:265" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <v>32</v>
       </c>
@@ -4509,8 +5334,50 @@
       <c r="HG19" s="1">
         <v>16</v>
       </c>
+      <c r="HL19" s="1">
+        <v>16</v>
+      </c>
+      <c r="HM19" s="1">
+        <v>17</v>
+      </c>
+      <c r="HO19" s="1">
+        <v>126</v>
+      </c>
+      <c r="HQ19" s="1">
+        <v>16</v>
+      </c>
+      <c r="HR19" s="1">
+        <v>10</v>
+      </c>
+      <c r="HT19" s="1">
+        <v>230</v>
+      </c>
+      <c r="HV19" s="7">
+        <v>16</v>
+      </c>
+      <c r="IA19" s="7">
+        <v>16</v>
+      </c>
+      <c r="IF19" s="7">
+        <v>16</v>
+      </c>
+      <c r="IK19" s="7">
+        <v>16</v>
+      </c>
+      <c r="IP19" s="1">
+        <v>16</v>
+      </c>
+      <c r="IU19" s="1">
+        <v>16</v>
+      </c>
+      <c r="IZ19" s="1">
+        <v>16</v>
+      </c>
+      <c r="JE19" s="1">
+        <v>16</v>
+      </c>
     </row>
-    <row r="20" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:265" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <v>55</v>
       </c>
@@ -4682,8 +5549,50 @@
       <c r="HG20" s="1">
         <v>13</v>
       </c>
+      <c r="HL20" s="1">
+        <v>17</v>
+      </c>
+      <c r="HM20" s="1">
+        <v>19</v>
+      </c>
+      <c r="HO20" s="1">
+        <v>149</v>
+      </c>
+      <c r="HQ20" s="1">
+        <v>17</v>
+      </c>
+      <c r="HS20" s="1">
+        <v>4</v>
+      </c>
+      <c r="HT20" s="1">
+        <v>261</v>
+      </c>
+      <c r="HV20" s="7">
+        <v>17</v>
+      </c>
+      <c r="IA20" s="7">
+        <v>17</v>
+      </c>
+      <c r="IF20" s="7">
+        <v>17</v>
+      </c>
+      <c r="IK20" s="7">
+        <v>17</v>
+      </c>
+      <c r="IP20" s="1">
+        <v>17</v>
+      </c>
+      <c r="IU20" s="1">
+        <v>17</v>
+      </c>
+      <c r="IZ20" s="1">
+        <v>17</v>
+      </c>
+      <c r="JE20" s="1">
+        <v>17</v>
+      </c>
     </row>
-    <row r="21" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:265" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <v>35</v>
       </c>
@@ -4855,8 +5764,50 @@
       <c r="HG21" s="1">
         <v>14</v>
       </c>
+      <c r="HL21" s="1">
+        <v>18</v>
+      </c>
+      <c r="HM21" s="1">
+        <v>25</v>
+      </c>
+      <c r="HO21" s="1">
+        <v>110</v>
+      </c>
+      <c r="HQ21" s="1">
+        <v>18</v>
+      </c>
+      <c r="HR21" s="1">
+        <v>2</v>
+      </c>
+      <c r="HT21" s="1">
+        <v>275</v>
+      </c>
+      <c r="HV21" s="7">
+        <v>18</v>
+      </c>
+      <c r="IA21" s="7">
+        <v>18</v>
+      </c>
+      <c r="IF21" s="7">
+        <v>18</v>
+      </c>
+      <c r="IK21" s="7">
+        <v>18</v>
+      </c>
+      <c r="IP21" s="1">
+        <v>18</v>
+      </c>
+      <c r="IU21" s="1">
+        <v>18</v>
+      </c>
+      <c r="IZ21" s="1">
+        <v>18</v>
+      </c>
+      <c r="JE21" s="1">
+        <v>18</v>
+      </c>
     </row>
-    <row r="22" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
         <v>19</v>
       </c>
@@ -5025,8 +5976,50 @@
       <c r="HF22" s="1">
         <v>6</v>
       </c>
+      <c r="HL22" s="1">
+        <v>19</v>
+      </c>
+      <c r="HN22" s="1">
+        <v>15</v>
+      </c>
+      <c r="HO22" s="1">
+        <v>144</v>
+      </c>
+      <c r="HQ22" s="1">
+        <v>19</v>
+      </c>
+      <c r="HR22" s="1">
+        <v>5</v>
+      </c>
+      <c r="HT22" s="1">
+        <v>253</v>
+      </c>
+      <c r="HV22" s="7">
+        <v>19</v>
+      </c>
+      <c r="IA22" s="7">
+        <v>19</v>
+      </c>
+      <c r="IF22" s="7">
+        <v>19</v>
+      </c>
+      <c r="IK22" s="7">
+        <v>19</v>
+      </c>
+      <c r="IP22" s="1">
+        <v>19</v>
+      </c>
+      <c r="IU22" s="1">
+        <v>19</v>
+      </c>
+      <c r="IZ22" s="1">
+        <v>19</v>
+      </c>
+      <c r="JE22" s="1">
+        <v>19</v>
+      </c>
     </row>
-    <row r="23" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
         <v>20</v>
       </c>
@@ -5189,8 +6182,44 @@
       <c r="HG23" s="1">
         <v>11</v>
       </c>
+      <c r="HL23" s="1">
+        <v>20</v>
+      </c>
+      <c r="HN23" s="1">
+        <v>8</v>
+      </c>
+      <c r="HO23" s="1">
+        <v>156</v>
+      </c>
+      <c r="HQ23" s="1">
+        <v>20</v>
+      </c>
+      <c r="HV23" s="7">
+        <v>20</v>
+      </c>
+      <c r="IA23" s="7">
+        <v>20</v>
+      </c>
+      <c r="IF23" s="7">
+        <v>20</v>
+      </c>
+      <c r="IK23" s="7">
+        <v>20</v>
+      </c>
+      <c r="IP23" s="1">
+        <v>20</v>
+      </c>
+      <c r="IU23" s="1">
+        <v>20</v>
+      </c>
+      <c r="IZ23" s="1">
+        <v>20</v>
+      </c>
+      <c r="JE23" s="1">
+        <v>20</v>
+      </c>
     </row>
-    <row r="24" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
         <v>21</v>
       </c>
@@ -5347,8 +6376,38 @@
       <c r="HE24" s="1">
         <v>21</v>
       </c>
+      <c r="HL24" s="1">
+        <v>21</v>
+      </c>
+      <c r="HQ24" s="1">
+        <v>21</v>
+      </c>
+      <c r="HV24" s="7">
+        <v>21</v>
+      </c>
+      <c r="IA24" s="7">
+        <v>21</v>
+      </c>
+      <c r="IF24" s="7">
+        <v>21</v>
+      </c>
+      <c r="IK24" s="7">
+        <v>21</v>
+      </c>
+      <c r="IP24" s="1">
+        <v>21</v>
+      </c>
+      <c r="IU24" s="1">
+        <v>21</v>
+      </c>
+      <c r="IZ24" s="1">
+        <v>21</v>
+      </c>
+      <c r="JE24" s="1">
+        <v>21</v>
+      </c>
     </row>
-    <row r="25" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
         <v>22</v>
       </c>
@@ -5505,8 +6564,38 @@
       <c r="HE25" s="1">
         <v>22</v>
       </c>
+      <c r="HL25" s="1">
+        <v>22</v>
+      </c>
+      <c r="HQ25" s="1">
+        <v>22</v>
+      </c>
+      <c r="HV25" s="7">
+        <v>22</v>
+      </c>
+      <c r="IA25" s="7">
+        <v>22</v>
+      </c>
+      <c r="IF25" s="7">
+        <v>22</v>
+      </c>
+      <c r="IK25" s="7">
+        <v>22</v>
+      </c>
+      <c r="IP25" s="1">
+        <v>22</v>
+      </c>
+      <c r="IU25" s="1">
+        <v>22</v>
+      </c>
+      <c r="IZ25" s="1">
+        <v>22</v>
+      </c>
+      <c r="JE25" s="1">
+        <v>22</v>
+      </c>
     </row>
-    <row r="26" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <v>23</v>
       </c>
@@ -5660,8 +6749,38 @@
       <c r="HE26" s="1">
         <v>23</v>
       </c>
+      <c r="HL26" s="1">
+        <v>23</v>
+      </c>
+      <c r="HQ26" s="1">
+        <v>23</v>
+      </c>
+      <c r="HV26" s="7">
+        <v>23</v>
+      </c>
+      <c r="IA26" s="7">
+        <v>23</v>
+      </c>
+      <c r="IF26" s="7">
+        <v>23</v>
+      </c>
+      <c r="IK26" s="7">
+        <v>23</v>
+      </c>
+      <c r="IP26" s="1">
+        <v>23</v>
+      </c>
+      <c r="IU26" s="1">
+        <v>23</v>
+      </c>
+      <c r="IZ26" s="1">
+        <v>23</v>
+      </c>
+      <c r="JE26" s="1">
+        <v>23</v>
+      </c>
     </row>
-    <row r="27" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>24</v>
       </c>
@@ -5815,8 +6934,38 @@
       <c r="HE27" s="1">
         <v>24</v>
       </c>
+      <c r="HL27" s="1">
+        <v>24</v>
+      </c>
+      <c r="HQ27" s="1">
+        <v>24</v>
+      </c>
+      <c r="HV27" s="7">
+        <v>24</v>
+      </c>
+      <c r="IA27" s="7">
+        <v>24</v>
+      </c>
+      <c r="IF27" s="7">
+        <v>24</v>
+      </c>
+      <c r="IK27" s="7">
+        <v>24</v>
+      </c>
+      <c r="IP27" s="1">
+        <v>24</v>
+      </c>
+      <c r="IU27" s="1">
+        <v>24</v>
+      </c>
+      <c r="IZ27" s="1">
+        <v>24</v>
+      </c>
+      <c r="JE27" s="1">
+        <v>24</v>
+      </c>
     </row>
-    <row r="28" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E28" s="1">
         <v>25</v>
       </c>
@@ -5970,8 +7119,38 @@
       <c r="HE28" s="1">
         <v>25</v>
       </c>
+      <c r="HL28" s="1">
+        <v>25</v>
+      </c>
+      <c r="HQ28" s="1">
+        <v>25</v>
+      </c>
+      <c r="HV28" s="7">
+        <v>25</v>
+      </c>
+      <c r="IA28" s="7">
+        <v>25</v>
+      </c>
+      <c r="IF28" s="7">
+        <v>25</v>
+      </c>
+      <c r="IK28" s="7">
+        <v>25</v>
+      </c>
+      <c r="IP28" s="1">
+        <v>25</v>
+      </c>
+      <c r="IU28" s="1">
+        <v>25</v>
+      </c>
+      <c r="IZ28" s="1">
+        <v>25</v>
+      </c>
+      <c r="JE28" s="1">
+        <v>25</v>
+      </c>
     </row>
-    <row r="29" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <v>26</v>
       </c>
@@ -6098,8 +7277,38 @@
       <c r="HE29" s="1">
         <v>26</v>
       </c>
+      <c r="HL29" s="1">
+        <v>26</v>
+      </c>
+      <c r="HQ29" s="1">
+        <v>26</v>
+      </c>
+      <c r="HV29" s="7">
+        <v>26</v>
+      </c>
+      <c r="IA29" s="7">
+        <v>26</v>
+      </c>
+      <c r="IF29" s="7">
+        <v>26</v>
+      </c>
+      <c r="IK29" s="7">
+        <v>26</v>
+      </c>
+      <c r="IP29" s="1">
+        <v>26</v>
+      </c>
+      <c r="IU29" s="1">
+        <v>26</v>
+      </c>
+      <c r="IZ29" s="1">
+        <v>26</v>
+      </c>
+      <c r="JE29" s="1">
+        <v>26</v>
+      </c>
     </row>
-    <row r="30" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E30" s="1">
         <v>27</v>
       </c>
@@ -6226,8 +7435,38 @@
       <c r="HE30" s="1">
         <v>27</v>
       </c>
+      <c r="HL30" s="1">
+        <v>27</v>
+      </c>
+      <c r="HQ30" s="1">
+        <v>27</v>
+      </c>
+      <c r="HV30" s="7">
+        <v>27</v>
+      </c>
+      <c r="IA30" s="7">
+        <v>27</v>
+      </c>
+      <c r="IF30" s="7">
+        <v>27</v>
+      </c>
+      <c r="IK30" s="7">
+        <v>27</v>
+      </c>
+      <c r="IP30" s="1">
+        <v>27</v>
+      </c>
+      <c r="IU30" s="1">
+        <v>27</v>
+      </c>
+      <c r="IZ30" s="1">
+        <v>27</v>
+      </c>
+      <c r="JE30" s="1">
+        <v>27</v>
+      </c>
     </row>
-    <row r="31" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E31" s="1">
         <v>28</v>
       </c>
@@ -6354,8 +7593,38 @@
       <c r="HE31" s="1">
         <v>28</v>
       </c>
+      <c r="HL31" s="1">
+        <v>28</v>
+      </c>
+      <c r="HQ31" s="1">
+        <v>28</v>
+      </c>
+      <c r="HV31" s="7">
+        <v>28</v>
+      </c>
+      <c r="IA31" s="7">
+        <v>28</v>
+      </c>
+      <c r="IF31" s="7">
+        <v>28</v>
+      </c>
+      <c r="IK31" s="7">
+        <v>28</v>
+      </c>
+      <c r="IP31" s="1">
+        <v>28</v>
+      </c>
+      <c r="IU31" s="1">
+        <v>28</v>
+      </c>
+      <c r="IZ31" s="1">
+        <v>28</v>
+      </c>
+      <c r="JE31" s="1">
+        <v>28</v>
+      </c>
     </row>
-    <row r="32" spans="2:216" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:265" x14ac:dyDescent="0.25">
       <c r="E32" s="1">
         <v>29</v>
       </c>
@@ -6482,8 +7751,38 @@
       <c r="HE32" s="1">
         <v>29</v>
       </c>
+      <c r="HL32" s="1">
+        <v>29</v>
+      </c>
+      <c r="HQ32" s="1">
+        <v>29</v>
+      </c>
+      <c r="HV32" s="7">
+        <v>29</v>
+      </c>
+      <c r="IA32" s="7">
+        <v>29</v>
+      </c>
+      <c r="IF32" s="7">
+        <v>29</v>
+      </c>
+      <c r="IK32" s="7">
+        <v>29</v>
+      </c>
+      <c r="IP32" s="1">
+        <v>29</v>
+      </c>
+      <c r="IU32" s="1">
+        <v>29</v>
+      </c>
+      <c r="IZ32" s="1">
+        <v>29</v>
+      </c>
+      <c r="JE32" s="1">
+        <v>29</v>
+      </c>
     </row>
-    <row r="33" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:268" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <v>30</v>
       </c>
@@ -6610,8 +7909,38 @@
       <c r="HE33" s="1">
         <v>30</v>
       </c>
+      <c r="HL33" s="1">
+        <v>30</v>
+      </c>
+      <c r="HQ33" s="1">
+        <v>30</v>
+      </c>
+      <c r="HV33" s="7">
+        <v>30</v>
+      </c>
+      <c r="IA33" s="7">
+        <v>30</v>
+      </c>
+      <c r="IF33" s="7">
+        <v>30</v>
+      </c>
+      <c r="IK33" s="7">
+        <v>30</v>
+      </c>
+      <c r="IP33" s="1">
+        <v>30</v>
+      </c>
+      <c r="IU33" s="1">
+        <v>30</v>
+      </c>
+      <c r="IZ33" s="1">
+        <v>30</v>
+      </c>
+      <c r="JE33" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="34" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:268" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -7178,9 +8507,159 @@
         <f>AVERAGE(HH3:HH33)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="HL34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="HM34" s="1">
+        <f>SUM(HM3:HM33)</f>
+        <v>96</v>
+      </c>
+      <c r="HN34" s="1">
+        <f>SUM(HN3:HN33)</f>
+        <v>55</v>
+      </c>
+      <c r="HO34" s="1">
+        <f>AVERAGE(HO3:HO33)</f>
+        <v>134</v>
+      </c>
+      <c r="HQ34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="HR34" s="1">
+        <f>SUM(HR3:HR33)</f>
+        <v>60</v>
+      </c>
+      <c r="HS34" s="1">
+        <f>SUM(HS3:HS33)</f>
+        <v>17</v>
+      </c>
+      <c r="HT34" s="1">
+        <f>AVERAGE(HT3:HT33)</f>
+        <v>225.75</v>
+      </c>
+      <c r="HV34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="HW34" s="7">
+        <f>SUM(HW3:HW33)</f>
+        <v>131</v>
+      </c>
+      <c r="HX34" s="7">
+        <f>SUM(HX3:HX33)</f>
+        <v>0</v>
+      </c>
+      <c r="HY34" s="7" t="e">
+        <f>AVERAGE(HY3:HY33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IA34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="IB34" s="7">
+        <f>SUM(IB3:IB33)</f>
+        <v>37</v>
+      </c>
+      <c r="IC34" s="7">
+        <f>SUM(IC3:IC33)</f>
+        <v>165</v>
+      </c>
+      <c r="ID34" s="7" t="e">
+        <f>AVERAGE(ID3:ID33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IF34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="IG34" s="7">
+        <f>SUM(IG3:IG33)</f>
+        <v>136</v>
+      </c>
+      <c r="IH34" s="7">
+        <f>SUM(IH3:IH33)</f>
+        <v>0</v>
+      </c>
+      <c r="II34" s="7" t="e">
+        <f>AVERAGE(II3:II33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IK34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="IL34" s="7">
+        <f>SUM(IL3:IL33)</f>
+        <v>0</v>
+      </c>
+      <c r="IM34" s="7">
+        <f>SUM(IM3:IM33)</f>
+        <v>49</v>
+      </c>
+      <c r="IN34" s="7" t="e">
+        <f>AVERAGE(IN3:IN33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IP34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="IQ34" s="1">
+        <f>SUM(IQ3:IQ33)</f>
+        <v>0</v>
+      </c>
+      <c r="IR34" s="1">
+        <f>SUM(IR3:IR33)</f>
+        <v>0</v>
+      </c>
+      <c r="IS34" s="1" t="e">
+        <f>AVERAGE(IS3:IS33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IU34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="IV34" s="1">
+        <f>SUM(IV3:IV33)</f>
+        <v>0</v>
+      </c>
+      <c r="IW34" s="1">
+        <f>SUM(IW3:IW33)</f>
+        <v>0</v>
+      </c>
+      <c r="IX34" s="1" t="e">
+        <f>AVERAGE(IX3:IX33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IZ34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="JA34" s="1">
+        <f>SUM(JA3:JA33)</f>
+        <v>0</v>
+      </c>
+      <c r="JB34" s="1">
+        <f>SUM(JB3:JB33)</f>
+        <v>0</v>
+      </c>
+      <c r="JC34" s="1" t="e">
+        <f>AVERAGE(JC3:JC33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JE34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="JF34" s="1">
+        <f>SUM(JF3:JF33)</f>
+        <v>0</v>
+      </c>
+      <c r="JG34" s="1">
+        <f>SUM(JG3:JG33)</f>
+        <v>0</v>
+      </c>
+      <c r="JH34" s="1" t="e">
+        <f>AVERAGE(JH3:JH33)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="35" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="G35" s="10">
+    <row r="35" spans="1:268" x14ac:dyDescent="0.25">
+      <c r="G35" s="7">
         <f>(G34/4)*3</f>
         <v>130.5</v>
       </c>
@@ -7472,8 +8951,88 @@
         <f>(HG34/7)*5</f>
         <v>45.714285714285708</v>
       </c>
+      <c r="HM35" s="1">
+        <f>(HM34/7)*5</f>
+        <v>68.571428571428569</v>
+      </c>
+      <c r="HN35" s="1">
+        <f>(HN34/7)*5</f>
+        <v>39.285714285714285</v>
+      </c>
+      <c r="HR35" s="1">
+        <f>(HR34/7)*5</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="HS35" s="1">
+        <f>(HS34/7)*5</f>
+        <v>12.142857142857142</v>
+      </c>
+      <c r="HW35" s="7">
+        <f>(HW34/7)*5</f>
+        <v>93.571428571428584</v>
+      </c>
+      <c r="HX35" s="7">
+        <f>(HX34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IB35" s="7">
+        <f>(IB34/7)*5</f>
+        <v>26.428571428571427</v>
+      </c>
+      <c r="IC35" s="7">
+        <f>(IC34/7)*5</f>
+        <v>117.85714285714286</v>
+      </c>
+      <c r="IG35" s="7">
+        <f>(IG34/7)*5</f>
+        <v>97.142857142857139</v>
+      </c>
+      <c r="IH35" s="7">
+        <f>(IH34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IL35" s="7">
+        <f>(IL34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IM35" s="7">
+        <f>(IM34/7)*5</f>
+        <v>35</v>
+      </c>
+      <c r="IQ35" s="1">
+        <f>(IQ34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IR35" s="1">
+        <f>(IR34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IV35" s="1">
+        <f>(IV34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="IW35" s="1">
+        <f>(IW34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="JA35" s="1">
+        <f>(JA34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="JB35" s="1">
+        <f>(JB34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="JF35" s="1">
+        <f>(JF34/7)*5</f>
+        <v>0</v>
+      </c>
+      <c r="JG35" s="1">
+        <f>(JG34/7)*5</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:216" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:268" x14ac:dyDescent="0.25">
       <c r="BZ36" s="1">
         <f>AVERAGE(BZ3:BZ33)</f>
         <v>6</v>
@@ -7722,9 +9281,194 @@
         <f>AVERAGE(EU3:EU33)</f>
         <v>7.6</v>
       </c>
+      <c r="HV36" s="7">
+        <f t="shared" ref="HV36:IN36" si="5">AVERAGE(HV3:HV33)</f>
+        <v>15.5</v>
+      </c>
+      <c r="HW36" s="7">
+        <f t="shared" si="5"/>
+        <v>43.666666666666664</v>
+      </c>
+      <c r="HX36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="HY36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="HZ36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IA36" s="7">
+        <f t="shared" si="5"/>
+        <v>15.5</v>
+      </c>
+      <c r="IB36" s="7">
+        <f t="shared" si="5"/>
+        <v>18.5</v>
+      </c>
+      <c r="IC36" s="7">
+        <f t="shared" si="5"/>
+        <v>12.692307692307692</v>
+      </c>
+      <c r="ID36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IE36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IF36" s="7">
+        <f t="shared" si="5"/>
+        <v>15.5</v>
+      </c>
+      <c r="IG36" s="7">
+        <f t="shared" si="5"/>
+        <v>27.2</v>
+      </c>
+      <c r="IH36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="II36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IJ36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IK36" s="7">
+        <f t="shared" si="5"/>
+        <v>15.5</v>
+      </c>
+      <c r="IL36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IM36" s="7">
+        <f t="shared" si="5"/>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="IN36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IP36" s="1">
+        <f t="shared" ref="IP36:JH36" si="6">AVERAGE(IP3:IP33)</f>
+        <v>15.5</v>
+      </c>
+      <c r="IQ36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IR36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IS36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IT36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IU36" s="1">
+        <f t="shared" si="6"/>
+        <v>15.5</v>
+      </c>
+      <c r="IV36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IW36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IX36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IY36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="IZ36" s="1">
+        <f t="shared" si="6"/>
+        <v>15.5</v>
+      </c>
+      <c r="JA36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JB36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JC36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JD36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JE36" s="1">
+        <f t="shared" si="6"/>
+        <v>15.5</v>
+      </c>
+      <c r="JF36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JG36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="JH36" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="49">
+    <mergeCell ref="IP1:IS1"/>
+    <mergeCell ref="IU1:IX1"/>
+    <mergeCell ref="IZ1:JC1"/>
+    <mergeCell ref="JE1:JH1"/>
+    <mergeCell ref="HV1:HY1"/>
+    <mergeCell ref="IA1:ID1"/>
+    <mergeCell ref="IF1:II1"/>
+    <mergeCell ref="IK1:IN1"/>
+    <mergeCell ref="DE1:DH1"/>
+    <mergeCell ref="HL1:HO1"/>
+    <mergeCell ref="HQ1:HT1"/>
+    <mergeCell ref="GP1:GS1"/>
+    <mergeCell ref="GU1:GX1"/>
+    <mergeCell ref="GZ1:HC1"/>
+    <mergeCell ref="GA1:GD1"/>
+    <mergeCell ref="GF1:GI1"/>
+    <mergeCell ref="GK1:GN1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="FH1:FK1"/>
+    <mergeCell ref="BI1:BL1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="BS1:BV1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CD1"/>
+    <mergeCell ref="CF1:CI1"/>
+    <mergeCell ref="CK1:CN1"/>
+    <mergeCell ref="CP1:CS1"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="CZ1:DC1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="HE1:HH1"/>
     <mergeCell ref="E1:H1"/>
@@ -7741,31 +9485,171 @@
     <mergeCell ref="EJ1:EM1"/>
     <mergeCell ref="DK1:DN1"/>
     <mergeCell ref="CU1:CX1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="FH1:FK1"/>
-    <mergeCell ref="BI1:BL1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="BS1:BV1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CD1"/>
-    <mergeCell ref="CF1:CI1"/>
-    <mergeCell ref="CK1:CN1"/>
-    <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="GP1:GS1"/>
-    <mergeCell ref="GU1:GX1"/>
-    <mergeCell ref="GZ1:HC1"/>
-    <mergeCell ref="GA1:GD1"/>
-    <mergeCell ref="GF1:GI1"/>
-    <mergeCell ref="GK1:GN1"/>
-    <mergeCell ref="CZ1:DC1"/>
-    <mergeCell ref="DE1:DH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <f>AVERAGE(B5:B26)</f>
+        <v>8.375</v>
+      </c>
+      <c r="C4" s="11" t="e">
+        <f t="shared" ref="C4:J4" si="0">AVERAGE(C5:C26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G4" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4</v>
+      </c>
+      <c r="I4" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>